<commit_message>
Se agregan tablas faltantes
</commit_message>
<xml_diff>
--- a/DiagramaDB.xlsx
+++ b/DiagramaDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisdavidlucio/Documents/gitHub_projects/GitHub/ProyectoController/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usert\Documents\Personal\Github\ProyectoController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA652A2-DC04-074A-B23F-77F809BDE272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2A0434-9219-4B2F-A623-293E834FC4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C5BDE85F-BCA1-FB42-B29A-4AFE7D908312}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5BDE85F-BCA1-FB42-B29A-4AFE7D908312}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -508,17 +508,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2753,29 +2753,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0631A18B-D189-684C-8496-02379FDB774E}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40:G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="22.625" customWidth="1"/>
+    <col min="9" max="9" width="18.625" customWidth="1"/>
+    <col min="10" max="10" width="16.375" customWidth="1"/>
+    <col min="11" max="11" width="17.125" customWidth="1"/>
+    <col min="12" max="12" width="28.375" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.875" customWidth="1"/>
+    <col min="15" max="15" width="22.375" customWidth="1"/>
+    <col min="16" max="16" width="13.875" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2794,7 +2794,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2813,30 +2813,30 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -2879,7 +2879,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -2918,7 +2918,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
@@ -2957,7 +2957,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -2996,7 +2996,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>10</v>
@@ -3035,7 +3035,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>13</v>
@@ -3074,7 +3074,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -3113,7 +3113,7 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -3142,7 +3142,7 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" ht="119" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>59</v>
@@ -3171,7 +3171,7 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3190,16 +3190,16 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -3211,7 +3211,7 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -3233,18 +3233,18 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -3285,7 +3285,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -3328,7 +3328,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
         <v>21</v>
@@ -3369,7 +3369,7 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
         <v>51</v>
@@ -3412,7 +3412,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -3441,7 +3441,7 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3460,7 +3460,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -3479,7 +3479,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3498,7 +3498,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -3519,30 +3519,30 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="11" t="s">
+      <c r="L25" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-    </row>
-    <row r="26" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="1" t="s">
         <v>0</v>
@@ -3588,7 +3588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="s">
         <v>57</v>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
         <v>62</v>
@@ -3668,7 +3668,7 @@
       </c>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="s">
         <v>65</v>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1" t="s">
         <v>3</v>
@@ -3752,7 +3752,7 @@
       </c>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="1" t="s">
         <v>68</v>
@@ -3770,11 +3770,11 @@
       <c r="G31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
       <c r="K31" s="5"/>
       <c r="L31" s="1" t="s">
         <v>68</v>
@@ -3796,7 +3796,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="2" t="s">
         <v>25</v>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="2" t="s">
         <v>73</v>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>82</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>84</v>
       </c>
@@ -3950,27 +3950,27 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G38" s="12" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G38" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="G39" s="11" t="s">
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G39" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-    </row>
-    <row r="40" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
         <v>0</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
         <v>94</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G42" s="1" t="s">
         <v>96</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G43" s="1" t="s">
         <v>45</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G44" s="1" t="s">
         <v>47</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G45" s="1" t="s">
         <v>0</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G46" s="2"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -4088,7 +4088,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G47" s="2"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -4109,14 +4109,15 @@
     <mergeCell ref="B25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="6">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega primera version de porton
</commit_message>
<xml_diff>
--- a/DiagramaDB.xlsx
+++ b/DiagramaDB.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usert\Documents\Personal\Github\ProyectoController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2A0434-9219-4B2F-A623-293E834FC4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AECA647-B5CE-4985-8EB6-786661DD02BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5BDE85F-BCA1-FB42-B29A-4AFE7D908312}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="111">
   <si>
     <t>nombre</t>
   </si>
@@ -348,6 +337,27 @@
   </si>
   <si>
     <t>Nombre de la persona o dato</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>uuid para identificar el porton</t>
+  </si>
+  <si>
+    <t>1 acceso total, 2 si solo puede ver los portones y 0 si no tiene ningun permiso</t>
+  </si>
+  <si>
+    <t>1 acceso total, 2 si solo puede ver los climas  y 0 si no tiene ningun permiso</t>
+  </si>
+  <si>
+    <t>0 si no puede agregar, 1 si puede agregar usuarios</t>
+  </si>
+  <si>
+    <t>1 es para saber si el porton esta activo</t>
+  </si>
+  <si>
+    <t>uuid para identificar de que porton o clima es esta instruccion</t>
   </si>
 </sst>
 </file>
@@ -389,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -478,11 +488,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -508,6 +529,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -524,7 +548,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="59">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1246,6 +1270,35 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2364,45 +2417,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}" name="Tabla2" displayName="Tabla2" ref="B4:G12" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}" name="Tabla2" displayName="Tabla2" ref="B4:G12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="B4:G12" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0E117ECB-B2BE-E444-A67E-AB752406DCB4}" name="nombre" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{8E692BCC-DCB9-7A41-BB4C-895C7E062EF6}" name="Tipo" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{F2CEF382-0414-C34A-BFDF-449781C89723}" name="PK" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{B473DF33-8912-BA43-97A5-5512C0A88AB1}" name="Nullable" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{8E484F5B-7117-FA43-A105-6F88F5B99A61}" name="FK" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{93BFFC49-9D2B-844E-9462-B12A29F0BD14}" name="Comentarios" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{0E117ECB-B2BE-E444-A67E-AB752406DCB4}" name="nombre" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{8E692BCC-DCB9-7A41-BB4C-895C7E062EF6}" name="Tipo" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{F2CEF382-0414-C34A-BFDF-449781C89723}" name="PK" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{B473DF33-8912-BA43-97A5-5512C0A88AB1}" name="Nullable" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{8E484F5B-7117-FA43-A105-6F88F5B99A61}" name="FK" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{93BFFC49-9D2B-844E-9462-B12A29F0BD14}" name="Comentarios" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}" name="Tabla24" displayName="Tabla24" ref="B15:G20" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="B15:G20" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}" name="Tabla24" displayName="Tabla24" ref="B15:G21" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+  <autoFilter ref="B15:G21" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{21AE7479-ECB4-C54C-8A3D-FFE43EB2F371}" name="nombre" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{0D79A7CC-61FD-EC42-9089-2CF159A78BDB}" name="Tipo" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{B6D7C3A6-008A-154F-BDE0-BCCD625CAB1B}" name="PK" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{1AA43FB1-C192-7C4C-A161-784F6B1FE6FA}" name="Nullable" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{B2B899F1-B01D-1944-8FBA-FA84D65FCBB2}" name="FK" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{13BB34BA-1F01-9D45-9D21-A8728D5519C9}" name="Comentarios" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{21AE7479-ECB4-C54C-8A3D-FFE43EB2F371}" name="nombre" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{0D79A7CC-61FD-EC42-9089-2CF159A78BDB}" name="Tipo" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{B6D7C3A6-008A-154F-BDE0-BCCD625CAB1B}" name="PK" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{1AA43FB1-C192-7C4C-A161-784F6B1FE6FA}" name="Nullable" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{B2B899F1-B01D-1944-8FBA-FA84D65FCBB2}" name="FK" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{13BB34BA-1F01-9D45-9D21-A8728D5519C9}" name="Comentarios" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{15C54008-32C7-0A4C-9C57-379BD4B8C775}" name="Tabla247" displayName="Tabla247" ref="J4:O10" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
-  <autoFilter ref="J4:O10" xr:uid="{15C54008-32C7-0A4C-9C57-379BD4B8C775}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C0F8A87D-2CBC-2E42-8E01-163145387525}" name="nombre" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{B57769AD-5C14-2540-B9F5-F8C17B881E19}" name="Tipo" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{3BCC004D-22AA-BA46-8471-468BD7DFFB12}" name="PK" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{EE648A7B-E271-C944-8D5B-DD904D1AC534}" name="Nullable" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{500328D1-C738-4047-82EB-D2ADBAEE745F}" name="FK" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{3BB50A08-A43C-8047-8894-DF8AA3AEAF21}" name="Comentarios" dataDxfId="31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{15C54008-32C7-0A4C-9C57-379BD4B8C775}" name="Tabla247" displayName="Tabla247" ref="J4:P10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="J4:P10" xr:uid="{15C54008-32C7-0A4C-9C57-379BD4B8C775}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C0F8A87D-2CBC-2E42-8E01-163145387525}" name="nombre" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{B57769AD-5C14-2540-B9F5-F8C17B881E19}" name="Tipo" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{3BCC004D-22AA-BA46-8471-468BD7DFFB12}" name="PK" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{EE648A7B-E271-C944-8D5B-DD904D1AC534}" name="Nullable" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{500328D1-C738-4047-82EB-D2ADBAEE745F}" name="FK" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{3BB50A08-A43C-8047-8894-DF8AA3AEAF21}" name="Comentarios" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{7CB03FF4-D35B-439B-A651-52C2CF7597EE}" name="Columna1" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2439,8 +2493,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}" name="Tabla24910" displayName="Tabla24910" ref="L26:R35" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="L26:R35" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}" name="Tabla24910" displayName="Tabla24910" ref="L26:R36" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="L26:R36" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{22AA9D7B-57AF-A340-A4E9-5F71CA9B5B80}" name="nombre" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{57330CE0-55D3-4046-A079-33152A89BD7E}" name="Tipo" dataDxfId="5"/>
@@ -2753,8 +2807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0631A18B-D189-684C-8496-02379FDB774E}">
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40:G45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2771,7 +2825,7 @@
     <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="14" max="14" width="17.875" customWidth="1"/>
     <col min="15" max="15" width="22.375" customWidth="1"/>
-    <col min="16" max="16" width="13.875" customWidth="1"/>
+    <col min="16" max="16" width="41.625" customWidth="1"/>
     <col min="17" max="17" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2815,24 +2869,24 @@
     </row>
     <row r="3" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -2876,7 +2930,9 @@
       <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -2915,7 +2971,7 @@
       <c r="O5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -2954,7 +3010,7 @@
       <c r="O6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -2993,7 +3049,9 @@
       <c r="O7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -3032,7 +3090,9 @@
       <c r="O8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -3071,7 +3131,9 @@
       <c r="O9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3110,7 +3172,7 @@
       <c r="O10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="3"/>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -3192,14 +3254,14 @@
     </row>
     <row r="14" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -3233,14 +3295,14 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
@@ -3441,14 +3503,24 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="7"/>
@@ -3521,26 +3593,26 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="9" t="s">
+      <c r="L25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
@@ -3628,7 +3700,7 @@
       </c>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
         <v>62</v>
@@ -3666,7 +3738,9 @@
       <c r="Q28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="R28" s="1"/>
+      <c r="R28" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
@@ -3770,11 +3844,11 @@
       <c r="G31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
       <c r="K31" s="5"/>
       <c r="L31" s="1" t="s">
         <v>68</v>
@@ -3950,25 +4024,44 @@
         <v>90</v>
       </c>
     </row>
+    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="L36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="R36" s="3"/>
+    </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">

</xml_diff>

<commit_message>
cambios para agregar usuarios
</commit_message>
<xml_diff>
--- a/DiagramaDB.xlsx
+++ b/DiagramaDB.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usert\Documents\Personal\Github\ProyectoController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Personal\Github\ProyectoController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AECA647-B5CE-4985-8EB6-786661DD02BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D44068-D911-48E2-974F-A14DAE2FB7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5BDE85F-BCA1-FB42-B29A-4AFE7D908312}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C5BDE85F-BCA1-FB42-B29A-4AFE7D908312}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lista cambios" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="126">
   <si>
     <t>nombre</t>
   </si>
@@ -358,6 +359,51 @@
   </si>
   <si>
     <t>uuid para identificar de que porton o clima es esta instruccion</t>
+  </si>
+  <si>
+    <t>id de la empresa a la que pertenece, su uso va principalmente en los usuarios de tipo admin, para que puedan asignar portones dependiendo el id de empresa</t>
+  </si>
+  <si>
+    <t>agregado 23 Jun</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Se agrega columna idEmpresa en la tabla ctUsuario</t>
+  </si>
+  <si>
+    <t>Se agrega num de version en la app para diferenciar</t>
+  </si>
+  <si>
+    <t>Version 2.1</t>
+  </si>
+  <si>
+    <t>Se modifica sp_valid_user para agregar campo idEmpresa</t>
+  </si>
+  <si>
+    <t>Se crea sp_get_users</t>
+  </si>
+  <si>
+    <t>Se modifica la app para mostrar todos los usuarios en una lista</t>
+  </si>
+  <si>
+    <t>App: ListUsers.tsx</t>
+  </si>
+  <si>
+    <t>App: Login.tsx</t>
+  </si>
+  <si>
+    <t>DB: sp_get_users</t>
+  </si>
+  <si>
+    <t>DB: ctUsuario, sp_valid_user</t>
+  </si>
+  <si>
+    <t>DB: tabla ctUsuario</t>
   </si>
 </sst>
 </file>
@@ -385,7 +431,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,6 +441,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -532,6 +584,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1986,7 +2050,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2139,13 +2203,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>243840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1320800</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>386080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2201,7 +2265,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2306,13 +2370,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>375920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>487680</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2367,7 +2431,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>365760</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2417,8 +2481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}" name="Tabla2" displayName="Tabla2" ref="B4:G12" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
-  <autoFilter ref="B4:G12" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}" name="Tabla2" displayName="Tabla2" ref="B4:G13" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+  <autoFilter ref="B4:G13" xr:uid="{B2243539-E401-CF41-B44D-40799321A622}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0E117ECB-B2BE-E444-A67E-AB752406DCB4}" name="nombre" dataDxfId="56"/>
     <tableColumn id="2" xr3:uid="{8E692BCC-DCB9-7A41-BB4C-895C7E062EF6}" name="Tipo" dataDxfId="55"/>
@@ -2432,8 +2496,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}" name="Tabla24" displayName="Tabla24" ref="B15:G21" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
-  <autoFilter ref="B15:G21" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}" name="Tabla24" displayName="Tabla24" ref="B16:G22" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47" totalsRowBorderDxfId="46">
+  <autoFilter ref="B16:G22" xr:uid="{7A933EE5-AA0B-DE45-8487-1031CDB8BFD1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{21AE7479-ECB4-C54C-8A3D-FFE43EB2F371}" name="nombre" dataDxfId="45"/>
     <tableColumn id="2" xr3:uid="{0D79A7CC-61FD-EC42-9089-2CF159A78BDB}" name="Tipo" dataDxfId="44"/>
@@ -2463,8 +2527,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8F959D9E-7A01-0A41-ACC7-07EF9C421F6C}" name="Tabla2478" displayName="Tabla2478" ref="J16:O19" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="J16:O19" xr:uid="{8F959D9E-7A01-0A41-ACC7-07EF9C421F6C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8F959D9E-7A01-0A41-ACC7-07EF9C421F6C}" name="Tabla2478" displayName="Tabla2478" ref="J17:O20" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="J17:O20" xr:uid="{8F959D9E-7A01-0A41-ACC7-07EF9C421F6C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7184B0F8-5729-FC4B-BC6F-10FC2C7103A2}" name="nombre" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{0D6B38F7-90EF-944C-8784-8BA045AC6804}" name="Tipo" dataDxfId="27"/>
@@ -2478,8 +2542,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{063AAC23-6BA8-7645-91B6-AD4A75B5C431}" name="Tabla249" displayName="Tabla249" ref="B26:G35" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B26:G35" xr:uid="{063AAC23-6BA8-7645-91B6-AD4A75B5C431}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{063AAC23-6BA8-7645-91B6-AD4A75B5C431}" name="Tabla249" displayName="Tabla249" ref="B27:G36" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B27:G36" xr:uid="{063AAC23-6BA8-7645-91B6-AD4A75B5C431}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{101875C0-7825-B04F-AED2-4AE6F5129E24}" name="nombre" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{0506F24A-FE90-2A47-8634-5BFDCEEEA537}" name="Tipo" dataDxfId="16"/>
@@ -2493,8 +2557,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}" name="Tabla24910" displayName="Tabla24910" ref="L26:R36" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="L26:R36" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}" name="Tabla24910" displayName="Tabla24910" ref="L27:R37" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="L27:R37" xr:uid="{9B9F6AAF-A839-A64D-9910-B21A4AABE0E1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{22AA9D7B-57AF-A340-A4E9-5F71CA9B5B80}" name="nombre" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{57330CE0-55D3-4046-A079-33152A89BD7E}" name="Tipo" dataDxfId="5"/>
@@ -2503,6 +2567,17 @@
     <tableColumn id="5" xr3:uid="{63DB205F-F96B-4F46-8699-444F3BDEE7D9}" name="FK" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{03B91359-35C4-9B42-B18F-DFE604B3E67F}" name="Comentarios" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{6F72BCF8-7D89-8D49-8585-B70CAA7B0357}" name="Columna1" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFBEE6AE-85C5-4861-BF23-711F336C94D0}" name="Tabla1" displayName="Tabla1" ref="A3:B8" totalsRowShown="0">
+  <autoFilter ref="A3:B8" xr:uid="{FFBEE6AE-85C5-4861-BF23-711F336C94D0}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3A2AE1C7-AF58-440B-AC96-379AC212C413}" name="Descripcion"/>
+    <tableColumn id="2" xr3:uid="{6F82448F-0BA6-464F-BDA9-5DDF51846A17}" name="Impacto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2805,10 +2880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0631A18B-D189-684C-8496-02379FDB774E}">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2869,24 +2944,24 @@
     </row>
     <row r="3" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -3233,14 +3308,26 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+    <row r="13" spans="1:17" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="s">
+        <v>111</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3252,16 +3339,14 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -3273,119 +3358,97 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="J16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="1" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -3393,10 +3456,10 @@
     <row r="18" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>7</v>
@@ -3404,20 +3467,22 @@
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>7</v>
@@ -3426,35 +3491,33 @@
         <v>7</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>15</v>
@@ -3463,63 +3526,77 @@
         <v>7</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
+      <c r="J20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="2" t="s">
-        <v>104</v>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4" t="s">
-        <v>110</v>
+      <c r="D21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -3532,14 +3609,24 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="7"/>
@@ -3553,20 +3640,20 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
@@ -3582,9 +3669,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="L24" s="5"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -3593,162 +3678,141 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="L25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R26" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="1" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P27" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="Q27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="R27" s="8"/>
-    </row>
-    <row r="28" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="P28" s="1"/>
       <c r="Q28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="R28" s="8"/>
+    </row>
+    <row r="29" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
@@ -3758,17 +3822,17 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>7</v>
@@ -3778,17 +3842,19 @@
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>7</v>
@@ -3796,21 +3862,19 @@
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="1" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>7</v>
@@ -3818,18 +3882,16 @@
       <c r="O30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="1" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
@@ -3840,18 +3902,18 @@
       <c r="E31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
+        <v>67</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="1" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>4</v>
@@ -3862,100 +3924,105 @@
       <c r="O31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P31" s="1"/>
+      <c r="P31" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="Q31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="B32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="R32" s="1"/>
-    </row>
-    <row r="33" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="L32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="2" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P33" s="3"/>
       <c r="Q33" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R33" s="3"/>
-    </row>
-    <row r="34" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
       <c r="B34" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>7</v>
@@ -3965,31 +4032,33 @@
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
       <c r="L34" s="2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="R34" s="3" t="s">
-        <v>90</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="R34" s="3"/>
     </row>
     <row r="35" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>63</v>
@@ -4002,10 +4071,10 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M35" s="3" t="s">
         <v>86</v>
@@ -4018,128 +4087,147 @@
       </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="G36" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="L36" s="2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="N36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="L37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="R36" s="3"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G38" s="11" t="s">
+      <c r="R37" s="3"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G39" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G39" s="10" t="s">
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G40" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="G42" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="J42" s="1" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G43" s="1" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G44" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>28</v>
@@ -4152,34 +4240,44 @@
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="G45" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="G46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G46" s="2"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G47" s="2"/>
@@ -4189,17 +4287,25 @@
       <c r="K47" s="3"/>
       <c r="L47" s="4"/>
     </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G48" s="2"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G40:L40"/>
     <mergeCell ref="G39:L39"/>
-    <mergeCell ref="G38:L38"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="L26:Q26"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
     <mergeCell ref="J3:O3"/>
-    <mergeCell ref="J15:O15"/>
-    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="J16:O16"/>
+    <mergeCell ref="B26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4213,4 +4319,79 @@
     <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0C1E63-FC59-4991-A949-51D6E5D0417B}">
+  <dimension ref="A2:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.75" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>